<commit_message>
Push to Git after VTiger changes done
</commit_message>
<xml_diff>
--- a/VtigerCRM/src/test/resources/TestData/VTiger.xlsx
+++ b/VtigerCRM/src/test/resources/TestData/VTiger.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Organization Name</t>
   </si>
@@ -31,19 +31,34 @@
   </si>
   <si>
     <t>ctcvthorg</t>
+  </si>
+  <si>
+    <t>Administrator - Organizations - vtiger CRM 5 - Commercial Open Source CRM</t>
+  </si>
+  <si>
+    <t>Expected Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Administrator - Contacts - vtiger CRM 5 - Commercial Open Source CRM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF201A1E"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,8 +81,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -362,56 +378,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
+    <col min="2" max="2" width="75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="64.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
VTiger project push after adding one more TestScript
</commit_message>
<xml_diff>
--- a/VtigerCRM/src/test/resources/TestData/VTiger.xlsx
+++ b/VtigerCRM/src/test/resources/TestData/VTiger.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="19875" windowHeight="7725" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="315" windowWidth="19875" windowHeight="7725"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Organization Name</t>
   </si>
@@ -40,6 +40,27 @@
   </si>
   <si>
     <t xml:space="preserve"> Administrator - Contacts - vtiger CRM 5 - Commercial Open Source CRM</t>
+  </si>
+  <si>
+    <t>Industry Names</t>
+  </si>
+  <si>
+    <t>Apparel</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Chemicals</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Flipkart</t>
   </si>
 </sst>
 </file>
@@ -378,32 +399,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="75" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -416,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>